<commit_message>
Updated Fasta files and prints to excel sheet.
</commit_message>
<xml_diff>
--- a/assets/XOLO_PTDB_Nomenclature.xlsx
+++ b/assets/XOLO_PTDB_Nomenclature.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crudnicky/Development/targetuploader/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F43535-C1AF-464D-913C-027B202F5C4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8A0B63-A5C3-F241-B34E-9E8B7EB3454F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="0" windowWidth="15840" windowHeight="21600" xr2:uid="{CCCF842F-453B-3647-8A0B-54DE93B664B8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{CCCF842F-453B-3647-8A0B-54DE93B664B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$47</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -936,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11387B1-20F5-B942-A26A-E0134A70B74A}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:F47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1344,7 +1347,7 @@
         <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="F20" t="s">
         <v>17</v>
@@ -1891,6 +1894,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F47" xr:uid="{5E95F934-8E18-284C-B94A-C197FDD6227B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>